<commit_message>
Modifica Master e tabella funzioni
</commit_message>
<xml_diff>
--- a/TabellaFunzioni.xlsx
+++ b/TabellaFunzioni.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Funzionalità</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve">DefaultState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
   </si>
   <si>
     <t xml:space="preserve">Accensione dei LED nella configurazione iniziale</t>
@@ -127,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -154,6 +157,13 @@
       <right/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -189,7 +199,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -219,6 +229,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -250,7 +264,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -272,7 +286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -283,58 +297,59 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="n">
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="n">
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
+      <c r="C6" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="8"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="9"/>
+        <v>14</v>
+      </c>
+      <c r="E9" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>